<commit_message>
perbaikan eksport import tapi masih di dashboard
</commit_message>
<xml_diff>
--- a/public/templates/template.xlsx
+++ b/public/templates/template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{417C0319-3680-47C4-B451-D01C98D766F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A673E47B-4B5D-4944-9D07-465A96BE6C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A735E6B2-4AB5-4203-B17A-80FEF7EF8D41}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{A735E6B2-4AB5-4203-B17A-80FEF7EF8D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>pertanyaan</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Pertanyaan</t>
+  </si>
+  <si>
+    <t>Aspek</t>
+  </si>
+  <si>
+    <t>Kriteria</t>
+  </si>
+  <si>
+    <t>aspek</t>
+  </si>
+  <si>
+    <t>kriteria</t>
+  </si>
+  <si>
+    <t>bobot</t>
   </si>
 </sst>
 </file>
@@ -77,8 +99,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,23 +441,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DAACFF-741B-4C53-B7E9-3878728E4CA3}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF67B4A-306D-481B-8BC4-FA11C610FB8E}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>